<commit_message>
go home take rest
</commit_message>
<xml_diff>
--- a/AR_Report.xlsx
+++ b/AR_Report.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="396">
   <si>
     <t>Action Request Report</t>
   </si>
@@ -1851,8 +1851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2056,9 +2056,7 @@
       <c r="K7" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="L7" s="17" t="s">
-        <v>44</v>
-      </c>
+      <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
       <c r="O7" s="17" t="s">

</xml_diff>

<commit_message>
go home this is friday
</commit_message>
<xml_diff>
--- a/AR_Report.xlsx
+++ b/AR_Report.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitMe\anphan2410\Working\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\An.Phan\GitMe\anphan2410\Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="396">
   <si>
     <t>Action Request Report</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>000034094</t>
   </si>
   <si>
     <t>3/15/2017 12:00:00 AM ICT</t>
@@ -1282,11 +1279,14 @@
     <t xml:space="preserve">yes co the chu
 </t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -1601,6 +1601,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1636,6 +1653,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1814,8 +1848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1890,7 +1924,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AI5" s="11" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="6" spans="1:35" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2002,7 +2036,7 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>38</v>
@@ -2154,7 +2188,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>69</v>
@@ -2301,14 +2335,12 @@
         <v>36</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="15" t="s">
-        <v>88</v>
-      </c>
+      <c r="D11" s="15"/>
       <c r="E11" s="15" t="s">
         <v>67</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G11" s="17" t="s">
         <v>80</v>
@@ -2317,10 +2349,10 @@
         <v>39</v>
       </c>
       <c r="I11" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="17" t="s">
         <v>89</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>90</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>42</v>
@@ -2331,7 +2363,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="P11" s="17" t="s">
         <v>45</v>
@@ -2340,7 +2372,7 @@
         <v>46</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="S11" s="17" t="s">
         <v>48</v>
@@ -2362,30 +2394,30 @@
       </c>
       <c r="AA11" s="17"/>
       <c r="AB11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="AC11" s="16" t="s">
         <v>93</v>
-      </c>
-      <c r="AC11" s="16" t="s">
-        <v>94</v>
       </c>
       <c r="AD11" s="17"/>
     </row>
     <row r="12" spans="1:35" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>97</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>98</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>39</v>
@@ -2394,7 +2426,7 @@
         <v>81</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>42</v>
@@ -2405,7 +2437,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P12" s="17" t="s">
         <v>45</v>
@@ -2414,7 +2446,7 @@
         <v>46</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S12" s="17" t="s">
         <v>48</v>
@@ -2436,25 +2468,25 @@
       </c>
       <c r="AA12" s="17"/>
       <c r="AB12" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="AC12" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="AC12" s="16" t="s">
-        <v>103</v>
       </c>
       <c r="AD12" s="17"/>
     </row>
     <row r="13" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="16" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>80</v>
@@ -2466,7 +2498,7 @@
         <v>58</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>42</v>
@@ -2477,7 +2509,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P13" s="17" t="s">
         <v>45</v>
@@ -2486,7 +2518,7 @@
         <v>46</v>
       </c>
       <c r="R13" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S13" s="17" t="s">
         <v>48</v>
@@ -2508,25 +2540,25 @@
       </c>
       <c r="AA13" s="17"/>
       <c r="AB13" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="AC13" s="16" t="s">
         <v>109</v>
-      </c>
-      <c r="AC13" s="16" t="s">
-        <v>110</v>
       </c>
       <c r="AD13" s="17"/>
     </row>
     <row r="14" spans="1:35" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="16" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>80</v>
@@ -2535,10 +2567,10 @@
         <v>39</v>
       </c>
       <c r="I14" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="J14" s="17" t="s">
         <v>114</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>115</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>42</v>
@@ -2549,7 +2581,7 @@
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P14" s="17" t="s">
         <v>45</v>
@@ -2558,7 +2590,7 @@
         <v>46</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>48</v>
@@ -2580,29 +2612,29 @@
       </c>
       <c r="AA14" s="17"/>
       <c r="AB14" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="AC14" s="16" t="s">
         <v>116</v>
-      </c>
-      <c r="AC14" s="16" t="s">
-        <v>117</v>
       </c>
       <c r="AD14" s="17"/>
     </row>
     <row r="15" spans="1:35" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>57</v>
@@ -2614,7 +2646,7 @@
         <v>40</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>42</v>
@@ -2625,7 +2657,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="P15" s="17" t="s">
         <v>45</v>
@@ -2634,7 +2666,7 @@
         <v>46</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="S15" s="17" t="s">
         <v>38</v>
@@ -2643,7 +2675,7 @@
         <v>63</v>
       </c>
       <c r="U15" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="V15" s="17"/>
       <c r="W15" s="17"/>
@@ -2656,27 +2688,27 @@
       </c>
       <c r="AA15" s="17"/>
       <c r="AB15" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="AC15" s="16" t="s">
         <v>125</v>
-      </c>
-      <c r="AC15" s="16" t="s">
-        <v>126</v>
       </c>
       <c r="AD15" s="17"/>
     </row>
     <row r="16" spans="1:35" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G16" s="17" t="s">
         <v>80</v>
@@ -2685,10 +2717,10 @@
         <v>39</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>42</v>
@@ -2699,7 +2731,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P16" s="17" t="s">
         <v>45</v>
@@ -2708,7 +2740,7 @@
         <v>46</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="S16" s="17" t="s">
         <v>48</v>
@@ -2730,29 +2762,29 @@
       </c>
       <c r="AA16" s="17"/>
       <c r="AB16" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="AC16" s="16" t="s">
         <v>133</v>
-      </c>
-      <c r="AC16" s="16" t="s">
-        <v>134</v>
       </c>
       <c r="AD16" s="17"/>
     </row>
     <row r="17" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>69</v>
@@ -2761,19 +2793,19 @@
         <v>39</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>45</v>
@@ -2782,7 +2814,7 @@
         <v>46</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S17" s="17" t="s">
         <v>38</v>
@@ -2791,7 +2823,7 @@
         <v>63</v>
       </c>
       <c r="U17" s="17" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V17" s="17"/>
       <c r="W17" s="17"/>
@@ -2804,39 +2836,39 @@
       </c>
       <c r="AA17" s="17"/>
       <c r="AB17" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="AC17" s="16" t="s">
         <v>143</v>
-      </c>
-      <c r="AC17" s="16" t="s">
-        <v>144</v>
       </c>
       <c r="AD17" s="17"/>
     </row>
     <row r="18" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="16" t="s">
+        <v>146</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>147</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>148</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>149</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>150</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>42</v>
@@ -2847,7 +2879,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P18" s="17" t="s">
         <v>45</v>
@@ -2856,7 +2888,7 @@
         <v>46</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S18" s="17" t="s">
         <v>48</v>
@@ -2878,39 +2910,39 @@
       </c>
       <c r="AA18" s="17"/>
       <c r="AB18" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="AC18" s="16" t="s">
         <v>153</v>
-      </c>
-      <c r="AC18" s="16" t="s">
-        <v>154</v>
       </c>
       <c r="AD18" s="17"/>
     </row>
     <row r="19" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>157</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>158</v>
       </c>
       <c r="H19" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="J19" s="17" t="s">
         <v>159</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>160</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>42</v>
@@ -2921,7 +2953,7 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="P19" s="17" t="s">
         <v>45</v>
@@ -2930,7 +2962,7 @@
         <v>46</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="S19" s="17" t="s">
         <v>48</v>
@@ -2952,25 +2984,25 @@
       </c>
       <c r="AA19" s="17"/>
       <c r="AB19" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="AC19" s="16" t="s">
         <v>161</v>
-      </c>
-      <c r="AC19" s="16" t="s">
-        <v>162</v>
       </c>
       <c r="AD19" s="17"/>
     </row>
     <row r="20" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="16" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>69</v>
@@ -2979,10 +3011,10 @@
         <v>39</v>
       </c>
       <c r="I20" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="J20" s="17" t="s">
         <v>166</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>167</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>42</v>
@@ -2993,7 +3025,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P20" s="17" t="s">
         <v>45</v>
@@ -3002,7 +3034,7 @@
         <v>46</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="S20" s="17" t="s">
         <v>48</v>
@@ -3024,25 +3056,25 @@
       </c>
       <c r="AA20" s="17"/>
       <c r="AB20" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="AC20" s="16" t="s">
         <v>170</v>
-      </c>
-      <c r="AC20" s="16" t="s">
-        <v>171</v>
       </c>
       <c r="AD20" s="17"/>
     </row>
     <row r="21" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="16" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>38</v>
@@ -3054,7 +3086,7 @@
         <v>40</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>42</v>
@@ -3065,7 +3097,7 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="P21" s="17" t="s">
         <v>45</v>
@@ -3074,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S21" s="17" t="s">
         <v>48</v>
@@ -3096,39 +3128,39 @@
       </c>
       <c r="AA21" s="17"/>
       <c r="AB21" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="AC21" s="16" t="s">
         <v>178</v>
-      </c>
-      <c r="AC21" s="16" t="s">
-        <v>179</v>
       </c>
       <c r="AD21" s="17"/>
     </row>
     <row r="22" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>182</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>183</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="J22" s="17" t="s">
         <v>184</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>185</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>42</v>
@@ -3139,7 +3171,7 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="P22" s="17" t="s">
         <v>45</v>
@@ -3148,7 +3180,7 @@
         <v>46</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="S22" s="17" t="s">
         <v>48</v>
@@ -3170,25 +3202,25 @@
       </c>
       <c r="AA22" s="17"/>
       <c r="AB22" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="AC22" s="16" t="s">
         <v>188</v>
-      </c>
-      <c r="AC22" s="16" t="s">
-        <v>189</v>
       </c>
       <c r="AD22" s="17"/>
     </row>
     <row r="23" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>38</v>
@@ -3200,7 +3232,7 @@
         <v>40</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="K23" s="17" t="s">
         <v>42</v>
@@ -3211,7 +3243,7 @@
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P23" s="17" t="s">
         <v>45</v>
@@ -3220,7 +3252,7 @@
         <v>46</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S23" s="17" t="s">
         <v>48</v>
@@ -3242,37 +3274,37 @@
       </c>
       <c r="AA23" s="17"/>
       <c r="AB23" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="AC23" s="16" t="s">
         <v>196</v>
-      </c>
-      <c r="AC23" s="16" t="s">
-        <v>197</v>
       </c>
       <c r="AD23" s="17"/>
     </row>
     <row r="24" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="16" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I24" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="J24" s="17" t="s">
         <v>201</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>202</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>42</v>
@@ -3283,7 +3315,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>45</v>
@@ -3292,7 +3324,7 @@
         <v>46</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S24" s="17" t="s">
         <v>48</v>
@@ -3314,25 +3346,25 @@
       </c>
       <c r="AA24" s="17"/>
       <c r="AB24" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="AC24" s="16" t="s">
         <v>205</v>
-      </c>
-      <c r="AC24" s="16" t="s">
-        <v>206</v>
       </c>
       <c r="AD24" s="17"/>
     </row>
     <row r="25" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="16" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>57</v>
@@ -3344,7 +3376,7 @@
         <v>40</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>42</v>
@@ -3355,7 +3387,7 @@
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="P25" s="17" t="s">
         <v>45</v>
@@ -3364,7 +3396,7 @@
         <v>46</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="S25" s="17" t="s">
         <v>48</v>
@@ -3386,25 +3418,25 @@
       </c>
       <c r="AA25" s="17"/>
       <c r="AB25" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="AC25" s="16" t="s">
         <v>213</v>
-      </c>
-      <c r="AC25" s="16" t="s">
-        <v>214</v>
       </c>
       <c r="AD25" s="17"/>
     </row>
     <row r="26" spans="1:30" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="16" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>57</v>
@@ -3416,20 +3448,20 @@
         <v>40</v>
       </c>
       <c r="J26" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="K26" s="17" t="s">
         <v>218</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>219</v>
       </c>
       <c r="L26" s="17" t="s">
         <v>43</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="P26" s="17" t="s">
         <v>45</v>
@@ -3438,7 +3470,7 @@
         <v>46</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="S26" s="17" t="s">
         <v>48</v>
@@ -3460,29 +3492,29 @@
       </c>
       <c r="AA26" s="17"/>
       <c r="AB26" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="AC26" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="AC26" s="16" t="s">
+      <c r="AD26" s="17" t="s">
         <v>223</v>
-      </c>
-      <c r="AD26" s="17" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="16" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>80</v>
@@ -3491,10 +3523,10 @@
         <v>39</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="K27" s="17" t="s">
         <v>42</v>
@@ -3505,7 +3537,7 @@
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
       <c r="O27" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P27" s="17" t="s">
         <v>45</v>
@@ -3514,7 +3546,7 @@
         <v>46</v>
       </c>
       <c r="R27" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="S27" s="17" t="s">
         <v>38</v>
@@ -3536,37 +3568,37 @@
       </c>
       <c r="AA27" s="17"/>
       <c r="AB27" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC27" s="16" t="s">
         <v>231</v>
-      </c>
-      <c r="AC27" s="16" t="s">
-        <v>232</v>
       </c>
       <c r="AD27" s="17"/>
     </row>
     <row r="28" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I28" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="J28" s="17" t="s">
         <v>236</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>237</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>42</v>
@@ -3577,7 +3609,7 @@
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
       <c r="O28" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P28" s="17" t="s">
         <v>45</v>
@@ -3586,10 +3618,10 @@
         <v>46</v>
       </c>
       <c r="R28" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="S28" s="17" t="s">
         <v>239</v>
-      </c>
-      <c r="S28" s="17" t="s">
-        <v>240</v>
       </c>
       <c r="T28" s="17" t="s">
         <v>49</v>
@@ -3608,50 +3640,50 @@
       </c>
       <c r="AA28" s="17"/>
       <c r="AB28" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC28" s="16" t="s">
         <v>241</v>
-      </c>
-      <c r="AC28" s="16" t="s">
-        <v>242</v>
       </c>
       <c r="AD28" s="17"/>
     </row>
     <row r="29" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>246</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>247</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
       <c r="O29" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="P29" s="17" t="s">
         <v>45</v>
@@ -3660,10 +3692,10 @@
         <v>46</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="S29" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="T29" s="17" t="s">
         <v>63</v>
@@ -3682,25 +3714,25 @@
       </c>
       <c r="AA29" s="17"/>
       <c r="AB29" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="AC29" s="16" t="s">
         <v>251</v>
-      </c>
-      <c r="AC29" s="16" t="s">
-        <v>252</v>
       </c>
       <c r="AD29" s="17"/>
     </row>
     <row r="30" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>38</v>
@@ -3709,10 +3741,10 @@
         <v>39</v>
       </c>
       <c r="I30" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="J30" s="17" t="s">
         <v>256</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>257</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>42</v>
@@ -3723,7 +3755,7 @@
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P30" s="17" t="s">
         <v>45</v>
@@ -3732,10 +3764,10 @@
         <v>46</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="S30" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T30" s="17" t="s">
         <v>49</v>
@@ -3754,27 +3786,27 @@
       </c>
       <c r="AA30" s="17"/>
       <c r="AB30" s="17" t="s">
+        <v>259</v>
+      </c>
+      <c r="AC30" s="16" t="s">
         <v>260</v>
-      </c>
-      <c r="AC30" s="16" t="s">
-        <v>261</v>
       </c>
       <c r="AD30" s="17"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>69</v>
@@ -3783,21 +3815,21 @@
         <v>39</v>
       </c>
       <c r="I31" s="17" t="s">
+        <v>264</v>
+      </c>
+      <c r="J31" s="17" t="s">
         <v>265</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>266</v>
       </c>
       <c r="K31" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
       <c r="O31" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="P31" s="17" t="s">
         <v>45</v>
@@ -3806,7 +3838,7 @@
         <v>46</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="S31" s="17" t="s">
         <v>69</v>
@@ -3828,37 +3860,37 @@
       </c>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="AC31" s="16" t="s">
         <v>268</v>
-      </c>
-      <c r="AC31" s="16" t="s">
-        <v>269</v>
       </c>
       <c r="AD31" s="17"/>
     </row>
     <row r="32" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="16" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I32" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="J32" s="17" t="s">
         <v>273</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>274</v>
       </c>
       <c r="K32" s="17" t="s">
         <v>42</v>
@@ -3869,7 +3901,7 @@
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
       <c r="O32" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P32" s="17" t="s">
         <v>45</v>
@@ -3878,10 +3910,10 @@
         <v>46</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="S32" s="17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="T32" s="17" t="s">
         <v>49</v>
@@ -3900,39 +3932,39 @@
       </c>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="AC32" s="16" t="s">
         <v>277</v>
-      </c>
-      <c r="AC32" s="16" t="s">
-        <v>278</v>
       </c>
       <c r="AD32" s="17"/>
     </row>
     <row r="33" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="16" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="J33" s="17" t="s">
         <v>282</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>283</v>
       </c>
       <c r="K33" s="17" t="s">
         <v>42</v>
@@ -3943,7 +3975,7 @@
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
       <c r="O33" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="P33" s="17" t="s">
         <v>45</v>
@@ -3952,7 +3984,7 @@
         <v>46</v>
       </c>
       <c r="R33" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S33" s="17" t="s">
         <v>38</v>
@@ -3965,7 +3997,7 @@
       </c>
       <c r="V33" s="17"/>
       <c r="W33" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="X33" s="17"/>
       <c r="Y33" s="17" t="s">
@@ -3976,25 +4008,25 @@
       </c>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17" t="s">
+        <v>286</v>
+      </c>
+      <c r="AC33" s="16" t="s">
         <v>287</v>
-      </c>
-      <c r="AC33" s="16" t="s">
-        <v>288</v>
       </c>
       <c r="AD33" s="17"/>
     </row>
     <row r="34" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>57</v>
@@ -4003,10 +4035,10 @@
         <v>39</v>
       </c>
       <c r="I34" s="17" t="s">
+        <v>291</v>
+      </c>
+      <c r="J34" s="17" t="s">
         <v>292</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>293</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>42</v>
@@ -4017,7 +4049,7 @@
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P34" s="17" t="s">
         <v>45</v>
@@ -4026,7 +4058,7 @@
         <v>46</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S34" s="17" t="s">
         <v>48</v>
@@ -4048,27 +4080,27 @@
       </c>
       <c r="AA34" s="17"/>
       <c r="AB34" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="AC34" s="16" t="s">
         <v>296</v>
-      </c>
-      <c r="AC34" s="16" t="s">
-        <v>297</v>
       </c>
       <c r="AD34" s="17"/>
     </row>
     <row r="35" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G35" s="17" t="s">
         <v>80</v>
@@ -4077,10 +4109,10 @@
         <v>39</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="K35" s="17" t="s">
         <v>42</v>
@@ -4091,7 +4123,7 @@
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P35" s="17" t="s">
         <v>45</v>
@@ -4100,7 +4132,7 @@
         <v>46</v>
       </c>
       <c r="R35" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S35" s="17" t="s">
         <v>48</v>
@@ -4122,25 +4154,25 @@
       </c>
       <c r="AA35" s="17"/>
       <c r="AB35" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="AC35" s="16" t="s">
         <v>302</v>
-      </c>
-      <c r="AC35" s="16" t="s">
-        <v>303</v>
       </c>
       <c r="AD35" s="17"/>
     </row>
     <row r="36" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>38</v>
@@ -4149,10 +4181,10 @@
         <v>39</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K36" s="17" t="s">
         <v>42</v>
@@ -4163,7 +4195,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
       <c r="O36" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="P36" s="17" t="s">
         <v>45</v>
@@ -4172,7 +4204,7 @@
         <v>46</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="S36" s="17" t="s">
         <v>48</v>
@@ -4194,37 +4226,37 @@
       </c>
       <c r="AA36" s="17"/>
       <c r="AB36" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC36" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="AC36" s="16" t="s">
-        <v>309</v>
       </c>
       <c r="AD36" s="17"/>
     </row>
     <row r="37" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="16" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I37" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="J37" s="17" t="s">
         <v>313</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>314</v>
       </c>
       <c r="K37" s="17" t="s">
         <v>42</v>
@@ -4235,7 +4267,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
       <c r="O37" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P37" s="17" t="s">
         <v>45</v>
@@ -4244,7 +4276,7 @@
         <v>46</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S37" s="17" t="s">
         <v>48</v>
@@ -4266,25 +4298,25 @@
       </c>
       <c r="AA37" s="17"/>
       <c r="AB37" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="AC37" s="16" t="s">
         <v>317</v>
-      </c>
-      <c r="AC37" s="16" t="s">
-        <v>318</v>
       </c>
       <c r="AD37" s="17"/>
     </row>
     <row r="38" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E38" s="15"/>
       <c r="F38" s="16" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>57</v>
@@ -4293,10 +4325,10 @@
         <v>39</v>
       </c>
       <c r="I38" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="J38" s="17" t="s">
         <v>322</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>323</v>
       </c>
       <c r="K38" s="17" t="s">
         <v>42</v>
@@ -4307,7 +4339,7 @@
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P38" s="17" t="s">
         <v>45</v>
@@ -4316,7 +4348,7 @@
         <v>46</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="S38" s="17" t="s">
         <v>48</v>
@@ -4338,25 +4370,25 @@
       </c>
       <c r="AA38" s="17"/>
       <c r="AB38" s="17" t="s">
+        <v>323</v>
+      </c>
+      <c r="AC38" s="16" t="s">
         <v>324</v>
-      </c>
-      <c r="AC38" s="16" t="s">
-        <v>325</v>
       </c>
       <c r="AD38" s="17"/>
     </row>
     <row r="39" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="16" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>69</v>
@@ -4365,10 +4397,10 @@
         <v>39</v>
       </c>
       <c r="I39" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="J39" s="17" t="s">
         <v>329</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>330</v>
       </c>
       <c r="K39" s="17" t="s">
         <v>42</v>
@@ -4379,7 +4411,7 @@
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="P39" s="17" t="s">
         <v>45</v>
@@ -4388,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="S39" s="17" t="s">
         <v>48</v>
@@ -4410,37 +4442,35 @@
       </c>
       <c r="AA39" s="17"/>
       <c r="AB39" s="17" t="s">
+        <v>332</v>
+      </c>
+      <c r="AC39" s="16" t="s">
         <v>333</v>
-      </c>
-      <c r="AC39" s="16" t="s">
-        <v>334</v>
       </c>
       <c r="AD39" s="17"/>
     </row>
     <row r="40" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="16" t="s">
-        <v>337</v>
-      </c>
-      <c r="G40" s="17" t="s">
-        <v>158</v>
-      </c>
+        <v>336</v>
+      </c>
+      <c r="G40" s="17"/>
       <c r="H40" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I40" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="J40" s="17" t="s">
         <v>338</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>339</v>
       </c>
       <c r="K40" s="17" t="s">
         <v>42</v>
@@ -4451,7 +4481,7 @@
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
       <c r="O40" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P40" s="17" t="s">
         <v>45</v>
@@ -4460,7 +4490,7 @@
         <v>46</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="S40" s="17" t="s">
         <v>48</v>
@@ -4482,37 +4512,37 @@
       </c>
       <c r="AA40" s="17"/>
       <c r="AB40" s="17" t="s">
+        <v>340</v>
+      </c>
+      <c r="AC40" s="16" t="s">
         <v>341</v>
-      </c>
-      <c r="AC40" s="16" t="s">
-        <v>342</v>
       </c>
       <c r="AD40" s="17"/>
     </row>
     <row r="41" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H41" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="I41" s="17" t="s">
         <v>345</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="J41" s="17" t="s">
         <v>346</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>347</v>
       </c>
       <c r="K41" s="17" t="s">
         <v>42</v>
@@ -4523,7 +4553,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P41" s="17" t="s">
         <v>45</v>
@@ -4532,7 +4562,7 @@
         <v>46</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S41" s="17" t="s">
         <v>48</v>
@@ -4554,25 +4584,25 @@
       </c>
       <c r="AA41" s="17"/>
       <c r="AB41" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="AC41" s="16" t="s">
         <v>349</v>
-      </c>
-      <c r="AC41" s="16" t="s">
-        <v>350</v>
       </c>
       <c r="AD41" s="17"/>
     </row>
     <row r="42" spans="1:30" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="16" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>38</v>
@@ -4581,10 +4611,10 @@
         <v>39</v>
       </c>
       <c r="I42" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="J42" s="17" t="s">
         <v>354</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>355</v>
       </c>
       <c r="K42" s="17" t="s">
         <v>42</v>
@@ -4595,7 +4625,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P42" s="17" t="s">
         <v>45</v>
@@ -4604,7 +4634,7 @@
         <v>46</v>
       </c>
       <c r="R42" s="17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="S42" s="17" t="s">
         <v>48</v>
@@ -4626,27 +4656,27 @@
       </c>
       <c r="AA42" s="17"/>
       <c r="AB42" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="AC42" s="16" t="s">
         <v>356</v>
-      </c>
-      <c r="AC42" s="16" t="s">
-        <v>357</v>
       </c>
       <c r="AD42" s="17"/>
     </row>
     <row r="43" spans="1:30" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E43" s="15" t="s">
         <v>87</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G43" s="17" t="s">
         <v>80</v>
@@ -4655,21 +4685,21 @@
         <v>39</v>
       </c>
       <c r="I43" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="J43" s="17" t="s">
         <v>361</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>362</v>
       </c>
       <c r="K43" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
       <c r="O43" s="17" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P43" s="17" t="s">
         <v>45</v>
@@ -4678,16 +4708,16 @@
         <v>46</v>
       </c>
       <c r="R43" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="S43" s="17" t="s">
         <v>364</v>
-      </c>
-      <c r="S43" s="17" t="s">
-        <v>365</v>
       </c>
       <c r="T43" s="17" t="s">
         <v>63</v>
       </c>
       <c r="U43" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="V43" s="17"/>
       <c r="W43" s="17"/>
@@ -4700,27 +4730,27 @@
       </c>
       <c r="AA43" s="17"/>
       <c r="AB43" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="AC43" s="16" t="s">
         <v>367</v>
       </c>
-      <c r="AC43" s="16" t="s">
-        <v>368</v>
-      </c>
       <c r="AD43" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E44" s="15"/>
       <c r="F44" s="16" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G44" s="17" t="s">
         <v>38</v>
@@ -4729,10 +4759,10 @@
         <v>39</v>
       </c>
       <c r="I44" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="J44" s="17" t="s">
         <v>371</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>372</v>
       </c>
       <c r="K44" s="17" t="s">
         <v>42</v>
@@ -4743,7 +4773,7 @@
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P44" s="17" t="s">
         <v>45</v>
@@ -4752,7 +4782,7 @@
         <v>46</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S44" s="17" t="s">
         <v>48</v>
@@ -4774,37 +4804,37 @@
       </c>
       <c r="AA44" s="17"/>
       <c r="AB44" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="AC44" s="16" t="s">
         <v>374</v>
-      </c>
-      <c r="AC44" s="16" t="s">
-        <v>375</v>
       </c>
       <c r="AD44" s="17"/>
     </row>
     <row r="45" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>38</v>
+        <v>395</v>
       </c>
       <c r="H45" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="J45" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="K45" s="17" t="s">
         <v>42</v>
@@ -4815,7 +4845,7 @@
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="P45" s="17" t="s">
         <v>45</v>
@@ -4824,7 +4854,7 @@
         <v>46</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="S45" s="17" t="s">
         <v>48</v>
@@ -4846,34 +4876,34 @@
       </c>
       <c r="AA45" s="17"/>
       <c r="AB45" s="17" t="s">
+        <v>379</v>
+      </c>
+      <c r="AC45" s="16" t="s">
         <v>380</v>
-      </c>
-      <c r="AC45" s="16" t="s">
-        <v>381</v>
       </c>
       <c r="AD45" s="17"/>
     </row>
     <row r="46" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="16" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17" t="s">
@@ -4885,7 +4915,7 @@
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P46" s="17" t="s">
         <v>45</v>
@@ -4894,7 +4924,7 @@
         <v>46</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="S46" s="17" t="s">
         <v>38</v>
@@ -4916,13 +4946,13 @@
       </c>
       <c r="AA46" s="17"/>
       <c r="AB46" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="AC46" s="16" t="s">
         <v>387</v>
       </c>
-      <c r="AC46" s="16" t="s">
-        <v>388</v>
-      </c>
       <c r="AD46" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -4948,10 +4978,10 @@
   <sheetData>
     <row r="2" spans="2:3" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
+        <v>388</v>
+      </c>
+      <c r="C2" t="s">
         <v>389</v>
-      </c>
-      <c r="C2" t="s">
-        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
thu 7 go home
</commit_message>
<xml_diff>
--- a/AR_Report.xlsx
+++ b/AR_Report.xlsx
@@ -269,9 +269,6 @@
 </t>
   </si>
   <si>
-    <t>TRUONG, THI (thtruong)</t>
-  </si>
-  <si>
     <t>3/30/2017 12:00:00 AM ICT</t>
   </si>
   <si>
@@ -1281,6 +1278,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>TRUONG, THI</t>
   </si>
 </sst>
 </file>
@@ -1849,7 +1849,7 @@
   <dimension ref="A1:AI46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1924,7 +1924,7 @@
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="AI5" s="11" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:35" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2036,7 +2036,7 @@
       </c>
       <c r="E7" s="15"/>
       <c r="F7" s="16" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="G7" s="17" t="s">
         <v>38</v>
@@ -2188,7 +2188,7 @@
         <v>35</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="G9" s="17" t="s">
         <v>69</v>
@@ -2269,16 +2269,16 @@
         <v>79</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H10" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I10" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="J10" s="17" t="s">
         <v>81</v>
-      </c>
-      <c r="J10" s="17" t="s">
-        <v>82</v>
       </c>
       <c r="K10" s="17" t="s">
         <v>42</v>
@@ -2289,7 +2289,7 @@
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
       <c r="O10" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="P10" s="17" t="s">
         <v>45</v>
@@ -2298,7 +2298,7 @@
         <v>46</v>
       </c>
       <c r="R10" s="17" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S10" s="17" t="s">
         <v>48</v>
@@ -2320,16 +2320,16 @@
       </c>
       <c r="AA10" s="17"/>
       <c r="AB10" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC10" s="16" t="s">
         <v>85</v>
-      </c>
-      <c r="AC10" s="16" t="s">
-        <v>86</v>
       </c>
       <c r="AD10" s="17"/>
     </row>
     <row r="11" spans="1:35" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>36</v>
@@ -2340,19 +2340,19 @@
         <v>67</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H11" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I11" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="J11" s="17" t="s">
         <v>88</v>
-      </c>
-      <c r="J11" s="17" t="s">
-        <v>89</v>
       </c>
       <c r="K11" s="17" t="s">
         <v>42</v>
@@ -2363,7 +2363,7 @@
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
       <c r="O11" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="P11" s="17" t="s">
         <v>45</v>
@@ -2372,7 +2372,7 @@
         <v>46</v>
       </c>
       <c r="R11" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S11" s="17" t="s">
         <v>48</v>
@@ -2394,39 +2394,39 @@
       </c>
       <c r="AA11" s="17"/>
       <c r="AB11" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="AC11" s="16" t="s">
         <v>92</v>
-      </c>
-      <c r="AC11" s="16" t="s">
-        <v>93</v>
       </c>
       <c r="AD11" s="17"/>
     </row>
     <row r="12" spans="1:35" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E12" s="15"/>
       <c r="F12" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H12" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I12" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K12" s="17" t="s">
         <v>42</v>
@@ -2437,7 +2437,7 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
       <c r="O12" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P12" s="17" t="s">
         <v>45</v>
@@ -2446,7 +2446,7 @@
         <v>46</v>
       </c>
       <c r="R12" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="S12" s="17" t="s">
         <v>48</v>
@@ -2468,28 +2468,28 @@
       </c>
       <c r="AA12" s="17"/>
       <c r="AB12" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AC12" s="16" t="s">
         <v>101</v>
-      </c>
-      <c r="AC12" s="16" t="s">
-        <v>102</v>
       </c>
       <c r="AD12" s="17"/>
     </row>
     <row r="13" spans="1:35" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="15"/>
       <c r="D13" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E13" s="15"/>
       <c r="F13" s="16" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H13" s="17" t="s">
         <v>39</v>
@@ -2498,7 +2498,7 @@
         <v>58</v>
       </c>
       <c r="J13" s="17" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K13" s="17" t="s">
         <v>42</v>
@@ -2509,7 +2509,7 @@
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
       <c r="O13" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P13" s="17" t="s">
         <v>45</v>
@@ -2518,7 +2518,7 @@
         <v>46</v>
       </c>
       <c r="R13" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S13" s="17" t="s">
         <v>48</v>
@@ -2540,37 +2540,37 @@
       </c>
       <c r="AA13" s="17"/>
       <c r="AB13" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC13" s="16" t="s">
         <v>108</v>
-      </c>
-      <c r="AC13" s="16" t="s">
-        <v>109</v>
       </c>
       <c r="AD13" s="17"/>
     </row>
     <row r="14" spans="1:35" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="15"/>
       <c r="D14" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E14" s="15"/>
       <c r="F14" s="16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H14" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I14" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="J14" s="17" t="s">
-        <v>114</v>
       </c>
       <c r="K14" s="17" t="s">
         <v>42</v>
@@ -2581,7 +2581,7 @@
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
       <c r="O14" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="P14" s="17" t="s">
         <v>45</v>
@@ -2590,7 +2590,7 @@
         <v>46</v>
       </c>
       <c r="R14" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="S14" s="17" t="s">
         <v>48</v>
@@ -2612,29 +2612,29 @@
       </c>
       <c r="AA14" s="17"/>
       <c r="AB14" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AC14" s="16" t="s">
         <v>115</v>
-      </c>
-      <c r="AC14" s="16" t="s">
-        <v>116</v>
       </c>
       <c r="AD14" s="17"/>
     </row>
     <row r="15" spans="1:35" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>57</v>
@@ -2646,7 +2646,7 @@
         <v>40</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K15" s="17" t="s">
         <v>42</v>
@@ -2657,7 +2657,7 @@
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
       <c r="O15" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="P15" s="17" t="s">
         <v>45</v>
@@ -2666,7 +2666,7 @@
         <v>46</v>
       </c>
       <c r="R15" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="S15" s="17" t="s">
         <v>38</v>
@@ -2675,7 +2675,7 @@
         <v>63</v>
       </c>
       <c r="U15" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="V15" s="17"/>
       <c r="W15" s="17"/>
@@ -2688,39 +2688,39 @@
       </c>
       <c r="AA15" s="17"/>
       <c r="AB15" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AC15" s="16" t="s">
         <v>124</v>
-      </c>
-      <c r="AC15" s="16" t="s">
-        <v>125</v>
       </c>
       <c r="AD15" s="17"/>
     </row>
     <row r="16" spans="1:35" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="15"/>
       <c r="F16" s="16" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H16" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J16" s="17" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K16" s="17" t="s">
         <v>42</v>
@@ -2731,7 +2731,7 @@
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
       <c r="O16" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P16" s="17" t="s">
         <v>45</v>
@@ -2740,7 +2740,7 @@
         <v>46</v>
       </c>
       <c r="R16" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="S16" s="17" t="s">
         <v>48</v>
@@ -2762,29 +2762,29 @@
       </c>
       <c r="AA16" s="17"/>
       <c r="AB16" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC16" s="16" t="s">
         <v>132</v>
-      </c>
-      <c r="AC16" s="16" t="s">
-        <v>133</v>
       </c>
       <c r="AD16" s="17"/>
     </row>
     <row r="17" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="15" t="s">
         <v>54</v>
       </c>
       <c r="F17" s="16" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G17" s="17" t="s">
         <v>69</v>
@@ -2793,19 +2793,19 @@
         <v>39</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J17" s="17"/>
       <c r="K17" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L17" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
       <c r="O17" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="P17" s="17" t="s">
         <v>45</v>
@@ -2814,7 +2814,7 @@
         <v>46</v>
       </c>
       <c r="R17" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="S17" s="17" t="s">
         <v>38</v>
@@ -2823,7 +2823,7 @@
         <v>63</v>
       </c>
       <c r="U17" s="17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="V17" s="17"/>
       <c r="W17" s="17"/>
@@ -2836,39 +2836,39 @@
       </c>
       <c r="AA17" s="17"/>
       <c r="AB17" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="AC17" s="16" t="s">
         <v>142</v>
-      </c>
-      <c r="AC17" s="16" t="s">
-        <v>143</v>
       </c>
       <c r="AD17" s="17"/>
     </row>
     <row r="18" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C18" s="15"/>
       <c r="D18" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E18" s="15"/>
       <c r="F18" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="G18" s="17" t="s">
         <v>146</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>147</v>
       </c>
       <c r="H18" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I18" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="J18" s="17" t="s">
         <v>148</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>149</v>
       </c>
       <c r="K18" s="17" t="s">
         <v>42</v>
@@ -2879,7 +2879,7 @@
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
       <c r="O18" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P18" s="17" t="s">
         <v>45</v>
@@ -2888,7 +2888,7 @@
         <v>46</v>
       </c>
       <c r="R18" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S18" s="17" t="s">
         <v>48</v>
@@ -2910,39 +2910,39 @@
       </c>
       <c r="AA18" s="17"/>
       <c r="AB18" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC18" s="16" t="s">
         <v>152</v>
-      </c>
-      <c r="AC18" s="16" t="s">
-        <v>153</v>
       </c>
       <c r="AD18" s="17"/>
     </row>
     <row r="19" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" s="17" t="s">
         <v>156</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>157</v>
       </c>
       <c r="H19" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I19" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="J19" s="17" t="s">
         <v>158</v>
-      </c>
-      <c r="J19" s="17" t="s">
-        <v>159</v>
       </c>
       <c r="K19" s="17" t="s">
         <v>42</v>
@@ -2953,7 +2953,7 @@
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
       <c r="O19" s="17" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P19" s="17" t="s">
         <v>45</v>
@@ -2962,7 +2962,7 @@
         <v>46</v>
       </c>
       <c r="R19" s="17" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S19" s="17" t="s">
         <v>48</v>
@@ -2984,25 +2984,25 @@
       </c>
       <c r="AA19" s="17"/>
       <c r="AB19" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="AC19" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="AC19" s="16" t="s">
-        <v>161</v>
       </c>
       <c r="AD19" s="17"/>
     </row>
     <row r="20" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E20" s="15"/>
       <c r="F20" s="16" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G20" s="17" t="s">
         <v>69</v>
@@ -3011,10 +3011,10 @@
         <v>39</v>
       </c>
       <c r="I20" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="J20" s="17" t="s">
         <v>165</v>
-      </c>
-      <c r="J20" s="17" t="s">
-        <v>166</v>
       </c>
       <c r="K20" s="17" t="s">
         <v>42</v>
@@ -3025,7 +3025,7 @@
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
       <c r="O20" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P20" s="17" t="s">
         <v>45</v>
@@ -3034,7 +3034,7 @@
         <v>46</v>
       </c>
       <c r="R20" s="17" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="S20" s="17" t="s">
         <v>48</v>
@@ -3056,25 +3056,25 @@
       </c>
       <c r="AA20" s="17"/>
       <c r="AB20" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="AC20" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="AC20" s="16" t="s">
-        <v>170</v>
       </c>
       <c r="AD20" s="17"/>
     </row>
     <row r="21" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E21" s="15"/>
       <c r="F21" s="16" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G21" s="17" t="s">
         <v>38</v>
@@ -3086,7 +3086,7 @@
         <v>40</v>
       </c>
       <c r="J21" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K21" s="17" t="s">
         <v>42</v>
@@ -3097,7 +3097,7 @@
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
       <c r="O21" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P21" s="17" t="s">
         <v>45</v>
@@ -3106,7 +3106,7 @@
         <v>46</v>
       </c>
       <c r="R21" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S21" s="17" t="s">
         <v>48</v>
@@ -3128,39 +3128,39 @@
       </c>
       <c r="AA21" s="17"/>
       <c r="AB21" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="AC21" s="16" t="s">
         <v>177</v>
-      </c>
-      <c r="AC21" s="16" t="s">
-        <v>178</v>
       </c>
       <c r="AD21" s="17"/>
     </row>
     <row r="22" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E22" s="15"/>
       <c r="F22" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="17" t="s">
         <v>181</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>182</v>
       </c>
       <c r="H22" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I22" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="J22" s="17" t="s">
         <v>183</v>
-      </c>
-      <c r="J22" s="17" t="s">
-        <v>184</v>
       </c>
       <c r="K22" s="17" t="s">
         <v>42</v>
@@ -3171,7 +3171,7 @@
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
       <c r="O22" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="P22" s="17" t="s">
         <v>45</v>
@@ -3180,7 +3180,7 @@
         <v>46</v>
       </c>
       <c r="R22" s="17" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S22" s="17" t="s">
         <v>48</v>
@@ -3202,25 +3202,25 @@
       </c>
       <c r="AA22" s="17"/>
       <c r="AB22" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="AC22" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="AC22" s="16" t="s">
-        <v>188</v>
       </c>
       <c r="AD22" s="17"/>
     </row>
     <row r="23" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="15"/>
       <c r="D23" s="15" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E23" s="15"/>
       <c r="F23" s="16" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>38</v>
@@ -3232,7 +3232,7 @@
         <v>40</v>
       </c>
       <c r="J23" s="17" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="K23" s="17" t="s">
         <v>42</v>
@@ -3243,7 +3243,7 @@
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
       <c r="O23" s="17" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P23" s="17" t="s">
         <v>45</v>
@@ -3252,7 +3252,7 @@
         <v>46</v>
       </c>
       <c r="R23" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="S23" s="17" t="s">
         <v>48</v>
@@ -3274,37 +3274,37 @@
       </c>
       <c r="AA23" s="17"/>
       <c r="AB23" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC23" s="16" t="s">
         <v>195</v>
-      </c>
-      <c r="AC23" s="16" t="s">
-        <v>196</v>
       </c>
       <c r="AD23" s="17"/>
     </row>
     <row r="24" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="15"/>
       <c r="D24" s="15" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E24" s="15"/>
       <c r="F24" s="16" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H24" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I24" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="J24" s="17" t="s">
         <v>200</v>
-      </c>
-      <c r="J24" s="17" t="s">
-        <v>201</v>
       </c>
       <c r="K24" s="17" t="s">
         <v>42</v>
@@ -3315,7 +3315,7 @@
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
       <c r="O24" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="P24" s="17" t="s">
         <v>45</v>
@@ -3324,7 +3324,7 @@
         <v>46</v>
       </c>
       <c r="R24" s="17" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S24" s="17" t="s">
         <v>48</v>
@@ -3346,25 +3346,25 @@
       </c>
       <c r="AA24" s="17"/>
       <c r="AB24" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="AC24" s="16" t="s">
         <v>204</v>
-      </c>
-      <c r="AC24" s="16" t="s">
-        <v>205</v>
       </c>
       <c r="AD24" s="17"/>
     </row>
     <row r="25" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="15"/>
       <c r="D25" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E25" s="15"/>
       <c r="F25" s="16" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>57</v>
@@ -3376,7 +3376,7 @@
         <v>40</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="K25" s="17" t="s">
         <v>42</v>
@@ -3387,7 +3387,7 @@
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
       <c r="O25" s="17" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="P25" s="17" t="s">
         <v>45</v>
@@ -3396,7 +3396,7 @@
         <v>46</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S25" s="17" t="s">
         <v>48</v>
@@ -3418,25 +3418,25 @@
       </c>
       <c r="AA25" s="17"/>
       <c r="AB25" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="AC25" s="16" t="s">
         <v>212</v>
-      </c>
-      <c r="AC25" s="16" t="s">
-        <v>213</v>
       </c>
       <c r="AD25" s="17"/>
     </row>
     <row r="26" spans="1:30" ht="140.25" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B26" s="15"/>
       <c r="C26" s="15"/>
       <c r="D26" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E26" s="15"/>
       <c r="F26" s="16" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G26" s="17" t="s">
         <v>57</v>
@@ -3448,20 +3448,20 @@
         <v>40</v>
       </c>
       <c r="J26" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="K26" s="17" t="s">
         <v>217</v>
-      </c>
-      <c r="K26" s="17" t="s">
-        <v>218</v>
       </c>
       <c r="L26" s="17" t="s">
         <v>43</v>
       </c>
       <c r="M26" s="17"/>
       <c r="N26" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="P26" s="17" t="s">
         <v>45</v>
@@ -3470,7 +3470,7 @@
         <v>46</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="S26" s="17" t="s">
         <v>48</v>
@@ -3492,41 +3492,41 @@
       </c>
       <c r="AA26" s="17"/>
       <c r="AB26" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="AC26" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="AC26" s="16" t="s">
+      <c r="AD26" s="17" t="s">
         <v>222</v>
-      </c>
-      <c r="AD26" s="17" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="27" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="15"/>
       <c r="D27" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E27" s="15"/>
       <c r="F27" s="16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H27" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="K27" s="17" t="s">
         <v>42</v>
@@ -3537,7 +3537,7 @@
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
       <c r="O27" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="P27" s="17" t="s">
         <v>45</v>
@@ -3546,7 +3546,7 @@
         <v>46</v>
       </c>
       <c r="R27" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="S27" s="17" t="s">
         <v>38</v>
@@ -3568,37 +3568,37 @@
       </c>
       <c r="AA27" s="17"/>
       <c r="AB27" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="AC27" s="16" t="s">
         <v>230</v>
-      </c>
-      <c r="AC27" s="16" t="s">
-        <v>231</v>
       </c>
       <c r="AD27" s="17"/>
     </row>
     <row r="28" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B28" s="15"/>
       <c r="C28" s="15"/>
       <c r="D28" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E28" s="15"/>
       <c r="F28" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H28" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I28" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="J28" s="17" t="s">
         <v>235</v>
-      </c>
-      <c r="J28" s="17" t="s">
-        <v>236</v>
       </c>
       <c r="K28" s="17" t="s">
         <v>42</v>
@@ -3609,7 +3609,7 @@
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
       <c r="O28" s="17" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P28" s="17" t="s">
         <v>45</v>
@@ -3618,10 +3618,10 @@
         <v>46</v>
       </c>
       <c r="R28" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="S28" s="17" t="s">
         <v>238</v>
-      </c>
-      <c r="S28" s="17" t="s">
-        <v>239</v>
       </c>
       <c r="T28" s="17" t="s">
         <v>49</v>
@@ -3640,50 +3640,50 @@
       </c>
       <c r="AA28" s="17"/>
       <c r="AB28" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC28" s="16" t="s">
         <v>240</v>
-      </c>
-      <c r="AC28" s="16" t="s">
-        <v>241</v>
       </c>
       <c r="AD28" s="17"/>
     </row>
     <row r="29" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G29" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H29" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I29" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="J29" s="17" t="s">
         <v>245</v>
-      </c>
-      <c r="J29" s="17" t="s">
-        <v>246</v>
       </c>
       <c r="K29" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L29" s="17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
       <c r="O29" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P29" s="17" t="s">
         <v>45</v>
@@ -3692,10 +3692,10 @@
         <v>46</v>
       </c>
       <c r="R29" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="S29" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="T29" s="17" t="s">
         <v>63</v>
@@ -3714,25 +3714,25 @@
       </c>
       <c r="AA29" s="17"/>
       <c r="AB29" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="AC29" s="16" t="s">
         <v>250</v>
-      </c>
-      <c r="AC29" s="16" t="s">
-        <v>251</v>
       </c>
       <c r="AD29" s="17"/>
     </row>
     <row r="30" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E30" s="15"/>
       <c r="F30" s="16" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G30" s="17" t="s">
         <v>38</v>
@@ -3741,10 +3741,10 @@
         <v>39</v>
       </c>
       <c r="I30" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="J30" s="17" t="s">
         <v>255</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>256</v>
       </c>
       <c r="K30" s="17" t="s">
         <v>42</v>
@@ -3755,7 +3755,7 @@
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
       <c r="O30" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P30" s="17" t="s">
         <v>45</v>
@@ -3764,10 +3764,10 @@
         <v>46</v>
       </c>
       <c r="R30" s="17" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="S30" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T30" s="17" t="s">
         <v>49</v>
@@ -3786,27 +3786,27 @@
       </c>
       <c r="AA30" s="17"/>
       <c r="AB30" s="17" t="s">
+        <v>258</v>
+      </c>
+      <c r="AC30" s="16" t="s">
         <v>259</v>
-      </c>
-      <c r="AC30" s="16" t="s">
-        <v>260</v>
       </c>
       <c r="AD30" s="17"/>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E31" s="15" t="s">
         <v>35</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G31" s="17" t="s">
         <v>69</v>
@@ -3815,21 +3815,21 @@
         <v>39</v>
       </c>
       <c r="I31" s="17" t="s">
+        <v>263</v>
+      </c>
+      <c r="J31" s="17" t="s">
         <v>264</v>
-      </c>
-      <c r="J31" s="17" t="s">
-        <v>265</v>
       </c>
       <c r="K31" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L31" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
       <c r="O31" s="17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="P31" s="17" t="s">
         <v>45</v>
@@ -3838,7 +3838,7 @@
         <v>46</v>
       </c>
       <c r="R31" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="S31" s="17" t="s">
         <v>69</v>
@@ -3860,37 +3860,37 @@
       </c>
       <c r="AA31" s="17"/>
       <c r="AB31" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="AC31" s="16" t="s">
         <v>267</v>
-      </c>
-      <c r="AC31" s="16" t="s">
-        <v>268</v>
       </c>
       <c r="AD31" s="17"/>
     </row>
     <row r="32" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E32" s="15"/>
       <c r="F32" s="16" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="H32" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I32" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="J32" s="17" t="s">
         <v>272</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>273</v>
       </c>
       <c r="K32" s="17" t="s">
         <v>42</v>
@@ -3901,7 +3901,7 @@
       <c r="M32" s="17"/>
       <c r="N32" s="17"/>
       <c r="O32" s="17" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="P32" s="17" t="s">
         <v>45</v>
@@ -3910,10 +3910,10 @@
         <v>46</v>
       </c>
       <c r="R32" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="S32" s="17" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="T32" s="17" t="s">
         <v>49</v>
@@ -3932,39 +3932,39 @@
       </c>
       <c r="AA32" s="17"/>
       <c r="AB32" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="AC32" s="16" t="s">
         <v>276</v>
-      </c>
-      <c r="AC32" s="16" t="s">
-        <v>277</v>
       </c>
       <c r="AD32" s="17"/>
     </row>
     <row r="33" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="15" t="s">
         <v>6</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E33" s="15"/>
       <c r="F33" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H33" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I33" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="J33" s="17" t="s">
         <v>281</v>
-      </c>
-      <c r="J33" s="17" t="s">
-        <v>282</v>
       </c>
       <c r="K33" s="17" t="s">
         <v>42</v>
@@ -3975,7 +3975,7 @@
       <c r="M33" s="17"/>
       <c r="N33" s="17"/>
       <c r="O33" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="P33" s="17" t="s">
         <v>45</v>
@@ -3984,7 +3984,7 @@
         <v>46</v>
       </c>
       <c r="R33" s="17" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="S33" s="17" t="s">
         <v>38</v>
@@ -3997,7 +3997,7 @@
       </c>
       <c r="V33" s="17"/>
       <c r="W33" s="17" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="X33" s="17"/>
       <c r="Y33" s="17" t="s">
@@ -4008,25 +4008,25 @@
       </c>
       <c r="AA33" s="17"/>
       <c r="AB33" s="17" t="s">
+        <v>285</v>
+      </c>
+      <c r="AC33" s="16" t="s">
         <v>286</v>
-      </c>
-      <c r="AC33" s="16" t="s">
-        <v>287</v>
       </c>
       <c r="AD33" s="17"/>
     </row>
     <row r="34" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E34" s="15"/>
       <c r="F34" s="16" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="G34" s="17" t="s">
         <v>57</v>
@@ -4035,10 +4035,10 @@
         <v>39</v>
       </c>
       <c r="I34" s="17" t="s">
+        <v>290</v>
+      </c>
+      <c r="J34" s="17" t="s">
         <v>291</v>
-      </c>
-      <c r="J34" s="17" t="s">
-        <v>292</v>
       </c>
       <c r="K34" s="17" t="s">
         <v>42</v>
@@ -4049,7 +4049,7 @@
       <c r="M34" s="17"/>
       <c r="N34" s="17"/>
       <c r="O34" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P34" s="17" t="s">
         <v>45</v>
@@ -4058,7 +4058,7 @@
         <v>46</v>
       </c>
       <c r="R34" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S34" s="17" t="s">
         <v>48</v>
@@ -4080,39 +4080,39 @@
       </c>
       <c r="AA34" s="17"/>
       <c r="AB34" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="AC34" s="16" t="s">
         <v>295</v>
-      </c>
-      <c r="AC34" s="16" t="s">
-        <v>296</v>
       </c>
       <c r="AD34" s="17"/>
     </row>
     <row r="35" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>36</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E35" s="15"/>
       <c r="F35" s="16" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H35" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J35" s="17" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K35" s="17" t="s">
         <v>42</v>
@@ -4123,7 +4123,7 @@
       <c r="M35" s="17"/>
       <c r="N35" s="17"/>
       <c r="O35" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P35" s="17" t="s">
         <v>45</v>
@@ -4132,7 +4132,7 @@
         <v>46</v>
       </c>
       <c r="R35" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S35" s="17" t="s">
         <v>48</v>
@@ -4154,25 +4154,25 @@
       </c>
       <c r="AA35" s="17"/>
       <c r="AB35" s="17" t="s">
+        <v>300</v>
+      </c>
+      <c r="AC35" s="16" t="s">
         <v>301</v>
-      </c>
-      <c r="AC35" s="16" t="s">
-        <v>302</v>
       </c>
       <c r="AD35" s="17"/>
     </row>
     <row r="36" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E36" s="15"/>
       <c r="F36" s="16" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G36" s="17" t="s">
         <v>38</v>
@@ -4181,10 +4181,10 @@
         <v>39</v>
       </c>
       <c r="I36" s="17" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J36" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="K36" s="17" t="s">
         <v>42</v>
@@ -4195,7 +4195,7 @@
       <c r="M36" s="17"/>
       <c r="N36" s="17"/>
       <c r="O36" s="17" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="P36" s="17" t="s">
         <v>45</v>
@@ -4204,7 +4204,7 @@
         <v>46</v>
       </c>
       <c r="R36" s="17" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="S36" s="17" t="s">
         <v>48</v>
@@ -4226,37 +4226,37 @@
       </c>
       <c r="AA36" s="17"/>
       <c r="AB36" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC36" s="16" t="s">
         <v>307</v>
-      </c>
-      <c r="AC36" s="16" t="s">
-        <v>308</v>
       </c>
       <c r="AD36" s="17"/>
     </row>
     <row r="37" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E37" s="15"/>
       <c r="F37" s="16" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G37" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H37" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I37" s="17" t="s">
+        <v>311</v>
+      </c>
+      <c r="J37" s="17" t="s">
         <v>312</v>
-      </c>
-      <c r="J37" s="17" t="s">
-        <v>313</v>
       </c>
       <c r="K37" s="17" t="s">
         <v>42</v>
@@ -4267,7 +4267,7 @@
       <c r="M37" s="17"/>
       <c r="N37" s="17"/>
       <c r="O37" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P37" s="17" t="s">
         <v>45</v>
@@ -4276,7 +4276,7 @@
         <v>46</v>
       </c>
       <c r="R37" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S37" s="17" t="s">
         <v>48</v>
@@ -4298,25 +4298,25 @@
       </c>
       <c r="AA37" s="17"/>
       <c r="AB37" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="AC37" s="16" t="s">
         <v>316</v>
-      </c>
-      <c r="AC37" s="16" t="s">
-        <v>317</v>
       </c>
       <c r="AD37" s="17"/>
     </row>
     <row r="38" spans="1:30" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="15" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E38" s="15"/>
       <c r="F38" s="16" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="G38" s="17" t="s">
         <v>57</v>
@@ -4325,10 +4325,10 @@
         <v>39</v>
       </c>
       <c r="I38" s="17" t="s">
+        <v>320</v>
+      </c>
+      <c r="J38" s="17" t="s">
         <v>321</v>
-      </c>
-      <c r="J38" s="17" t="s">
-        <v>322</v>
       </c>
       <c r="K38" s="17" t="s">
         <v>42</v>
@@ -4339,7 +4339,7 @@
       <c r="M38" s="17"/>
       <c r="N38" s="17"/>
       <c r="O38" s="17" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P38" s="17" t="s">
         <v>45</v>
@@ -4348,7 +4348,7 @@
         <v>46</v>
       </c>
       <c r="R38" s="17" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="S38" s="17" t="s">
         <v>48</v>
@@ -4370,25 +4370,25 @@
       </c>
       <c r="AA38" s="17"/>
       <c r="AB38" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="AC38" s="16" t="s">
         <v>323</v>
-      </c>
-      <c r="AC38" s="16" t="s">
-        <v>324</v>
       </c>
       <c r="AD38" s="17"/>
     </row>
     <row r="39" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="15" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E39" s="15"/>
       <c r="F39" s="16" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G39" s="17" t="s">
         <v>69</v>
@@ -4397,10 +4397,10 @@
         <v>39</v>
       </c>
       <c r="I39" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="J39" s="17" t="s">
         <v>328</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>329</v>
       </c>
       <c r="K39" s="17" t="s">
         <v>42</v>
@@ -4411,7 +4411,7 @@
       <c r="M39" s="17"/>
       <c r="N39" s="17"/>
       <c r="O39" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="P39" s="17" t="s">
         <v>45</v>
@@ -4420,7 +4420,7 @@
         <v>46</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="S39" s="17" t="s">
         <v>48</v>
@@ -4442,35 +4442,35 @@
       </c>
       <c r="AA39" s="17"/>
       <c r="AB39" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="AC39" s="16" t="s">
         <v>332</v>
-      </c>
-      <c r="AC39" s="16" t="s">
-        <v>333</v>
       </c>
       <c r="AD39" s="17"/>
     </row>
     <row r="40" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="15" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E40" s="15"/>
       <c r="F40" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G40" s="17"/>
       <c r="H40" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I40" s="17" t="s">
+        <v>336</v>
+      </c>
+      <c r="J40" s="17" t="s">
         <v>337</v>
-      </c>
-      <c r="J40" s="17" t="s">
-        <v>338</v>
       </c>
       <c r="K40" s="17" t="s">
         <v>42</v>
@@ -4481,7 +4481,7 @@
       <c r="M40" s="17"/>
       <c r="N40" s="17"/>
       <c r="O40" s="17" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P40" s="17" t="s">
         <v>45</v>
@@ -4490,7 +4490,7 @@
         <v>46</v>
       </c>
       <c r="R40" s="17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="S40" s="17" t="s">
         <v>48</v>
@@ -4512,37 +4512,37 @@
       </c>
       <c r="AA40" s="17"/>
       <c r="AB40" s="17" t="s">
+        <v>339</v>
+      </c>
+      <c r="AC40" s="16" t="s">
         <v>340</v>
-      </c>
-      <c r="AC40" s="16" t="s">
-        <v>341</v>
       </c>
       <c r="AD40" s="17"/>
     </row>
     <row r="41" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="15" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E41" s="15"/>
       <c r="F41" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G41" s="17" t="s">
         <v>38</v>
       </c>
       <c r="H41" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="I41" s="17" t="s">
         <v>344</v>
       </c>
-      <c r="I41" s="17" t="s">
+      <c r="J41" s="17" t="s">
         <v>345</v>
-      </c>
-      <c r="J41" s="17" t="s">
-        <v>346</v>
       </c>
       <c r="K41" s="17" t="s">
         <v>42</v>
@@ -4553,7 +4553,7 @@
       <c r="M41" s="17"/>
       <c r="N41" s="17"/>
       <c r="O41" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P41" s="17" t="s">
         <v>45</v>
@@ -4562,7 +4562,7 @@
         <v>46</v>
       </c>
       <c r="R41" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S41" s="17" t="s">
         <v>48</v>
@@ -4584,25 +4584,25 @@
       </c>
       <c r="AA41" s="17"/>
       <c r="AB41" s="17" t="s">
+        <v>347</v>
+      </c>
+      <c r="AC41" s="16" t="s">
         <v>348</v>
-      </c>
-      <c r="AC41" s="16" t="s">
-        <v>349</v>
       </c>
       <c r="AD41" s="17"/>
     </row>
     <row r="42" spans="1:30" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="15" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E42" s="15"/>
       <c r="F42" s="16" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G42" s="17" t="s">
         <v>38</v>
@@ -4611,10 +4611,10 @@
         <v>39</v>
       </c>
       <c r="I42" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="J42" s="17" t="s">
         <v>353</v>
-      </c>
-      <c r="J42" s="17" t="s">
-        <v>354</v>
       </c>
       <c r="K42" s="17" t="s">
         <v>42</v>
@@ -4625,7 +4625,7 @@
       <c r="M42" s="17"/>
       <c r="N42" s="17"/>
       <c r="O42" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P42" s="17" t="s">
         <v>45</v>
@@ -4634,7 +4634,7 @@
         <v>46</v>
       </c>
       <c r="R42" s="17" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="S42" s="17" t="s">
         <v>48</v>
@@ -4656,50 +4656,50 @@
       </c>
       <c r="AA42" s="17"/>
       <c r="AB42" s="17" t="s">
+        <v>354</v>
+      </c>
+      <c r="AC42" s="16" t="s">
         <v>355</v>
-      </c>
-      <c r="AC42" s="16" t="s">
-        <v>356</v>
       </c>
       <c r="AD42" s="17"/>
     </row>
     <row r="43" spans="1:30" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="15" t="s">
+        <v>357</v>
+      </c>
+      <c r="E43" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="F43" s="16" t="s">
         <v>358</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F43" s="16" t="s">
-        <v>359</v>
-      </c>
       <c r="G43" s="17" t="s">
-        <v>80</v>
+        <v>395</v>
       </c>
       <c r="H43" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I43" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="J43" s="17" t="s">
         <v>360</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>361</v>
       </c>
       <c r="K43" s="17" t="s">
         <v>42</v>
       </c>
       <c r="L43" s="17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="M43" s="17"/>
       <c r="N43" s="17"/>
       <c r="O43" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="P43" s="17" t="s">
         <v>45</v>
@@ -4708,16 +4708,16 @@
         <v>46</v>
       </c>
       <c r="R43" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="S43" s="17" t="s">
         <v>363</v>
-      </c>
-      <c r="S43" s="17" t="s">
-        <v>364</v>
       </c>
       <c r="T43" s="17" t="s">
         <v>63</v>
       </c>
       <c r="U43" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="V43" s="17"/>
       <c r="W43" s="17"/>
@@ -4730,27 +4730,27 @@
       </c>
       <c r="AA43" s="17"/>
       <c r="AB43" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="AC43" s="16" t="s">
         <v>366</v>
       </c>
-      <c r="AC43" s="16" t="s">
-        <v>367</v>
-      </c>
       <c r="AD43" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E44" s="15"/>
       <c r="F44" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="G44" s="17" t="s">
         <v>38</v>
@@ -4759,10 +4759,10 @@
         <v>39</v>
       </c>
       <c r="I44" s="17" t="s">
+        <v>369</v>
+      </c>
+      <c r="J44" s="17" t="s">
         <v>370</v>
-      </c>
-      <c r="J44" s="17" t="s">
-        <v>371</v>
       </c>
       <c r="K44" s="17" t="s">
         <v>42</v>
@@ -4773,7 +4773,7 @@
       <c r="M44" s="17"/>
       <c r="N44" s="17"/>
       <c r="O44" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P44" s="17" t="s">
         <v>45</v>
@@ -4782,7 +4782,7 @@
         <v>46</v>
       </c>
       <c r="R44" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S44" s="17" t="s">
         <v>48</v>
@@ -4804,37 +4804,37 @@
       </c>
       <c r="AA44" s="17"/>
       <c r="AB44" s="17" t="s">
+        <v>372</v>
+      </c>
+      <c r="AC44" s="16" t="s">
         <v>373</v>
-      </c>
-      <c r="AC44" s="16" t="s">
-        <v>374</v>
       </c>
       <c r="AD44" s="17"/>
     </row>
     <row r="45" spans="1:30" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="15" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E45" s="15"/>
       <c r="F45" s="16" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H45" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I45" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="J45" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="K45" s="17" t="s">
         <v>42</v>
@@ -4845,7 +4845,7 @@
       <c r="M45" s="17"/>
       <c r="N45" s="17"/>
       <c r="O45" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="P45" s="17" t="s">
         <v>45</v>
@@ -4854,7 +4854,7 @@
         <v>46</v>
       </c>
       <c r="R45" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="S45" s="17" t="s">
         <v>48</v>
@@ -4876,34 +4876,34 @@
       </c>
       <c r="AA45" s="17"/>
       <c r="AB45" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="AC45" s="16" t="s">
         <v>379</v>
-      </c>
-      <c r="AC45" s="16" t="s">
-        <v>380</v>
       </c>
       <c r="AD45" s="17"/>
     </row>
     <row r="46" spans="1:30" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
       <c r="D46" s="15" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E46" s="15"/>
       <c r="F46" s="16" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H46" s="17" t="s">
         <v>39</v>
       </c>
       <c r="I46" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17" t="s">
@@ -4915,7 +4915,7 @@
       <c r="M46" s="17"/>
       <c r="N46" s="17"/>
       <c r="O46" s="17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="P46" s="17" t="s">
         <v>45</v>
@@ -4924,7 +4924,7 @@
         <v>46</v>
       </c>
       <c r="R46" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="S46" s="17" t="s">
         <v>38</v>
@@ -4946,13 +4946,13 @@
       </c>
       <c r="AA46" s="17"/>
       <c r="AB46" s="17" t="s">
+        <v>385</v>
+      </c>
+      <c r="AC46" s="16" t="s">
         <v>386</v>
       </c>
-      <c r="AC46" s="16" t="s">
-        <v>387</v>
-      </c>
       <c r="AD46" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -4978,10 +4978,10 @@
   <sheetData>
     <row r="2" spans="2:3" ht="409.5" x14ac:dyDescent="0.2">
       <c r="B2" s="21" t="s">
+        <v>387</v>
+      </c>
+      <c r="C2" t="s">
         <v>388</v>
-      </c>
-      <c r="C2" t="s">
-        <v>389</v>
       </c>
     </row>
   </sheetData>

</xml_diff>